<commit_message>
Current version of data in tables
</commit_message>
<xml_diff>
--- a/tables/dummy_table.xlsx
+++ b/tables/dummy_table.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/git/binary-neutron-stars-table/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D782318C-4B6A-FF41-8BB0-1C16AD49C1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E22A466-BBE0-DF49-A7F4-99A3C3E27D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{50F1C7DF-D392-F744-8597-796B657F6A2D}"/>
+    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{B4CAD46D-22B6-E948-AE2C-B74895AECFBB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="dummy_table" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,9 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
-  <si>
-    <t>N</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+  <si>
+    <t>#</t>
   </si>
   <si>
     <t>System</t>
@@ -170,64 +170,10 @@
     <t>Year</t>
   </si>
   <si>
-    <t>PSR J0453+1559</t>
-  </si>
-  <si>
-    <t>inf</t>
-  </si>
-  <si>
-    <t>a,b</t>
-  </si>
-  <si>
-    <t>PSR J0737-3039</t>
-  </si>
-  <si>
-    <t>PSR B1534+12</t>
-  </si>
-  <si>
-    <t>PSR J1756-2251</t>
-  </si>
-  <si>
     <t>PSR B1913+16</t>
   </si>
   <si>
-    <t>PSR J1913+1102</t>
-  </si>
-  <si>
-    <t>PSR J1757-1854</t>
-  </si>
-  <si>
-    <t>76, 130</t>
-  </si>
-  <si>
-    <t>b,c</t>
-  </si>
-  <si>
-    <t>PSR J1518+4904</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>PSR J1811-1736</t>
-  </si>
-  <si>
-    <t>PSR J1829+2456</t>
-  </si>
-  <si>
-    <t>PSR J1930-1852</t>
-  </si>
-  <si>
-    <t>PSR J1411+2551</t>
-  </si>
-  <si>
-    <t>b,e</t>
-  </si>
-  <si>
-    <t>PSR J1946+2052</t>
-  </si>
-  <si>
-    <t>c,f</t>
+    <t>a</t>
   </si>
   <si>
     <r>
@@ -246,13 +192,68 @@
     </r>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>PSR J0509+3801</t>
-  </si>
-  <si>
-    <t>g</t>
+    <t>b</t>
+  </si>
+  <si>
+    <t>PSR B1534+12</t>
+  </si>
+  <si>
+    <t>PSR J1518+4904</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
+    <t>PSR J1811-1736</t>
+  </si>
+  <si>
+    <t>PSR J0737-3039</t>
+  </si>
+  <si>
+    <t>PSR J1829+2456</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>PSR J1756-2251</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>PSR J1930-1852</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <r>
+      <t>PSR J0453+1559</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>PSR J1913+1102</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
   <si>
     <r>
@@ -280,7 +281,31 @@
     <t>0,86-1,36</t>
   </si>
   <si>
-    <t>h</t>
+    <t>p</t>
+  </si>
+  <si>
+    <t>PSR J1411+2551</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>PSR J1757-1854</t>
+  </si>
+  <si>
+    <t>76, 130</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>PSR J0509+3801</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>PSR J1946+2052</t>
   </si>
   <si>
     <r>
@@ -305,14 +330,29 @@
     <t>1,12-1,69</t>
   </si>
   <si>
-    <t>i</t>
+    <t>w</t>
+  </si>
+  <si>
+    <t>c-d</t>
+  </si>
+  <si>
+    <t>e-f</t>
+  </si>
+  <si>
+    <t>g-h</t>
+  </si>
+  <si>
+    <t>i-j</t>
+  </si>
+  <si>
+    <t>u-v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -345,6 +385,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -363,14 +411,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,7 +733,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4691A5C6-0091-1848-A044-6141160AE806}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069D6AA3-61BA-984C-82DA-7CD63676BD3E}">
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -737,66 +788,72 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>1.1754</v>
+        <v>1.2312000000000001</v>
       </c>
       <c r="D2">
-        <v>2.734</v>
+        <v>2.8279999999999998</v>
       </c>
       <c r="E2">
-        <v>1.5589999999999999</v>
+        <v>1.44</v>
       </c>
       <c r="F2">
-        <v>1.1739999999999999</v>
+        <v>1.389</v>
       </c>
       <c r="G2">
-        <v>45.8</v>
+        <v>59</v>
       </c>
       <c r="H2">
-        <v>4.0720000000000001</v>
+        <v>0.32300000000000001</v>
       </c>
       <c r="I2">
-        <v>0.113</v>
-      </c>
-      <c r="J2" t="s">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="J2">
+        <v>108</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>1.1805000000000001</v>
+      </c>
+      <c r="D3">
+        <v>2.7130000000000001</v>
+      </c>
+      <c r="E3">
+        <v>1.3580000000000001</v>
+      </c>
+      <c r="F3">
+        <v>1.3540000000000001</v>
+      </c>
+      <c r="G3">
+        <v>30.5</v>
+      </c>
+      <c r="H3">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="I3">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="J3">
+        <v>97</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>1.1253</v>
-      </c>
-      <c r="D3">
-        <v>2.5870000000000002</v>
-      </c>
-      <c r="E3">
-        <v>1.3380000000000001</v>
-      </c>
-      <c r="F3">
-        <v>1.2490000000000001</v>
-      </c>
-      <c r="G3">
-        <v>22.7</v>
-      </c>
-      <c r="H3">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="I3">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="J3">
-        <v>204</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
+      <c r="L3">
+        <v>1988</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -831,7 +888,10 @@
         <v>248</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>49</v>
+      </c>
+      <c r="L4">
+        <v>1991</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -841,32 +901,35 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
-        <v>1.1177999999999999</v>
+      <c r="C5" t="s">
+        <v>18</v>
       </c>
       <c r="D5">
-        <v>2.5710000000000002</v>
-      </c>
-      <c r="E5">
-        <v>1.341</v>
-      </c>
-      <c r="F5">
-        <v>1.23</v>
+        <v>2.718</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
       <c r="G5">
-        <v>28.5</v>
+        <v>40.9</v>
       </c>
       <c r="H5">
-        <v>0.32</v>
+        <v>8.6340000000000003</v>
       </c>
       <c r="I5">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="J5">
-        <v>443</v>
+        <v>0.249</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>14</v>
+        <v>50</v>
+      </c>
+      <c r="L5">
+        <v>1997</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -874,34 +937,37 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>1.2312000000000001</v>
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>2.8279999999999998</v>
-      </c>
-      <c r="E6">
-        <v>1.44</v>
-      </c>
-      <c r="F6">
-        <v>1.389</v>
+        <v>2.57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
       </c>
       <c r="G6">
-        <v>59</v>
+        <v>104.2</v>
       </c>
       <c r="H6">
-        <v>0.32300000000000001</v>
+        <v>18.779</v>
       </c>
       <c r="I6">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="J6">
-        <v>108</v>
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
+        <v>51</v>
+      </c>
+      <c r="L6">
+        <v>2001</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -909,34 +975,37 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>1.2467999999999999</v>
+        <v>1.1253</v>
       </c>
       <c r="D7">
-        <v>2.8887</v>
+        <v>2.5870000000000002</v>
       </c>
       <c r="E7">
-        <v>1.62</v>
+        <v>1.3380000000000001</v>
       </c>
       <c r="F7">
-        <v>1.27</v>
+        <v>1.2490000000000001</v>
       </c>
       <c r="G7">
-        <v>27.28</v>
+        <v>22.7</v>
       </c>
       <c r="H7">
-        <v>0.20599999999999999</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="I7">
-        <v>0.09</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="J7">
-        <v>2687</v>
+        <v>204</v>
       </c>
       <c r="K7" t="s">
-        <v>14</v>
+        <v>52</v>
+      </c>
+      <c r="L7">
+        <v>2003</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -944,34 +1013,37 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8">
-        <v>1.1893</v>
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
       </c>
       <c r="D8">
-        <v>2.7330000000000001</v>
-      </c>
-      <c r="E8">
-        <v>1.3380000000000001</v>
-      </c>
-      <c r="F8">
-        <v>1.395</v>
+        <v>2.59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
       </c>
       <c r="G8">
-        <v>21.5</v>
+        <v>41</v>
       </c>
       <c r="H8">
-        <v>0.183</v>
+        <v>1.1759999999999999</v>
       </c>
       <c r="I8">
-        <v>0.60599999999999998</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8">
+        <v>2004</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -979,34 +1051,37 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
         <v>24</v>
       </c>
+      <c r="C9">
+        <v>1.1177999999999999</v>
+      </c>
       <c r="D9">
-        <v>2.718</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
+        <v>2.5710000000000002</v>
+      </c>
+      <c r="E9">
+        <v>1.341</v>
+      </c>
+      <c r="F9">
+        <v>1.23</v>
       </c>
       <c r="G9">
-        <v>40.9</v>
+        <v>28.5</v>
       </c>
       <c r="H9">
-        <v>8.6340000000000003</v>
+        <v>0.32</v>
       </c>
       <c r="I9">
-        <v>0.249</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" t="s">
-        <v>14</v>
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="J9">
+        <v>443</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9">
+        <v>2005</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1014,69 +1089,75 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D10">
-        <v>2.57</v>
+        <v>2.59</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G10">
-        <v>104.2</v>
+        <v>185.5</v>
       </c>
       <c r="H10">
-        <v>18.779</v>
+        <v>45.06</v>
       </c>
       <c r="I10">
-        <v>0.82799999999999996</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>1.1754</v>
       </c>
       <c r="D11">
-        <v>2.59</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>24</v>
+        <v>2.734</v>
+      </c>
+      <c r="E11">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="F11">
+        <v>1.1739999999999999</v>
       </c>
       <c r="G11">
-        <v>41</v>
+        <v>45.8</v>
       </c>
       <c r="H11">
-        <v>1.1759999999999999</v>
+        <v>4.0720000000000001</v>
       </c>
       <c r="I11">
-        <v>0.13900000000000001</v>
+        <v>0.113</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11">
+        <v>2015</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1084,69 +1165,75 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>1.2467999999999999</v>
       </c>
       <c r="D12">
-        <v>2.59</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" t="s">
-        <v>24</v>
+        <v>2.8887</v>
+      </c>
+      <c r="E12">
+        <v>1.62</v>
+      </c>
+      <c r="F12">
+        <v>1.27</v>
       </c>
       <c r="G12">
-        <v>185.5</v>
+        <v>27.28</v>
       </c>
       <c r="H12">
-        <v>45.06</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="I12">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="J12" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.09</v>
+      </c>
+      <c r="J12">
+        <v>2687</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>2.5379999999999998</v>
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>1.1879999999999999</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13">
-        <v>62.4</v>
-      </c>
-      <c r="H13">
-        <v>2.6160000000000001</v>
-      </c>
-      <c r="I13">
-        <v>0.1699</v>
+        <v>35</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s">
+        <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13">
+        <v>2017</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1154,69 +1241,75 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14">
-        <v>1.0882000000000001</v>
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
       </c>
       <c r="D14">
-        <v>2.5</v>
-      </c>
-      <c r="E14">
-        <v>1.25</v>
-      </c>
-      <c r="F14">
-        <v>1.25</v>
+        <v>2.5379999999999998</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
       </c>
       <c r="G14">
-        <v>17</v>
+        <v>62.4</v>
       </c>
       <c r="H14">
-        <v>7.8E-2</v>
+        <v>2.6160000000000001</v>
       </c>
       <c r="I14">
-        <v>0.06</v>
-      </c>
-      <c r="J14">
-        <v>46</v>
-      </c>
-      <c r="K14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+        <v>0.1699</v>
+      </c>
+      <c r="J14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C15">
-        <v>1.1805000000000001</v>
+        <v>1.1893</v>
       </c>
       <c r="D15">
-        <v>2.7130000000000001</v>
+        <v>2.7330000000000001</v>
       </c>
       <c r="E15">
-        <v>1.3580000000000001</v>
+        <v>1.3380000000000001</v>
       </c>
       <c r="F15">
-        <v>1.3540000000000001</v>
+        <v>1.395</v>
       </c>
       <c r="G15">
-        <v>30.5</v>
+        <v>21.5</v>
       </c>
       <c r="H15">
-        <v>0.33500000000000002</v>
+        <v>0.183</v>
       </c>
       <c r="I15">
-        <v>0.68100000000000005</v>
-      </c>
-      <c r="J15">
-        <v>97</v>
-      </c>
-      <c r="K15" t="s">
-        <v>33</v>
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15">
+        <v>2018</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1224,7 +1317,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>1.2174</v>
@@ -1250,46 +1343,49 @@
       <c r="J16">
         <v>153</v>
       </c>
-      <c r="K16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="K16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C17">
-        <v>1.1879999999999999</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" t="s">
-        <v>24</v>
+        <v>1.0882000000000001</v>
+      </c>
+      <c r="D17">
+        <v>2.5</v>
+      </c>
+      <c r="E17">
+        <v>1.25</v>
+      </c>
+      <c r="F17">
+        <v>1.25</v>
+      </c>
+      <c r="G17">
+        <v>17</v>
+      </c>
+      <c r="H17">
+        <v>7.8E-2</v>
+      </c>
+      <c r="I17">
+        <v>0.06</v>
+      </c>
+      <c r="J17">
+        <v>46</v>
       </c>
       <c r="K17" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="L17">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="19" x14ac:dyDescent="0.2">
@@ -1297,7 +1393,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C18">
         <v>1.44</v>
@@ -1306,31 +1402,45 @@
         <v>3.4</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I18" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" t="s">
-        <v>44</v>
+        <v>18</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="L18">
         <v>2019</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" location="a" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - a" xr:uid="{69340366-5CF1-144E-9D52-97FEB34A0EAB}"/>
+    <hyperlink ref="K3" r:id="rId2" location="b" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - b" xr:uid="{A841F0E2-C4F2-1545-9CA1-C79DF8A4BB22}"/>
+    <hyperlink ref="K8" r:id="rId3" location="k" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - k" xr:uid="{F6218EAB-AF61-1245-9945-F6C9D8817BE1}"/>
+    <hyperlink ref="K9" r:id="rId4" location="l" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - l" xr:uid="{F6CEEC71-498B-9048-8E5A-095CB75FF22C}"/>
+    <hyperlink ref="K10" r:id="rId5" location="m" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - m" xr:uid="{60F52954-C194-864F-A120-B59044307F64}"/>
+    <hyperlink ref="K11" r:id="rId6" location="n" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - n" xr:uid="{D586A542-881F-214D-B06E-8601ACF6EB87}"/>
+    <hyperlink ref="K12" r:id="rId7" location="o" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - o" xr:uid="{C92F744F-3264-5A41-A724-32865B564718}"/>
+    <hyperlink ref="K13" r:id="rId8" location="p" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - p" xr:uid="{4AF3B618-76F4-9847-9F36-6E3B2148F196}"/>
+    <hyperlink ref="K14" r:id="rId9" location="q" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - q" xr:uid="{40341496-C6A8-BA47-B8E0-1BC06AD3986F}"/>
+    <hyperlink ref="K15" r:id="rId10" location="r" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - r" xr:uid="{285F8324-5B93-8243-AEE9-1CB8F6AC4B30}"/>
+    <hyperlink ref="K16" r:id="rId11" location="t" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - t" xr:uid="{46CB5D47-02E6-D044-9D2B-E6A857B19813}"/>
+    <hyperlink ref="K18" r:id="rId12" location="w" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - w" xr:uid="{EFAC2DA9-DD1F-5C45-8015-1EE190A9DD05}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More updates on table
</commit_message>
<xml_diff>
--- a/tables/dummy_table.xlsx
+++ b/tables/dummy_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/git/binary-neutron-stars-table/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CEAB6BAD-F8A9-2543-B910-F232A10229E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{952F5B6A-E1ED-1D45-9324-22A74F72AF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{FA939E62-D095-E54A-B717-B544DFC37576}"/>
+    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{2E5B3542-A0DE-C34A-9F8C-AF3FC35586CA}"/>
   </bookViews>
   <sheets>
     <sheet name="dummy_table" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
+    <t>#</t>
+  </si>
+  <si>
     <t>System</t>
   </si>
   <si>
@@ -176,27 +179,27 @@
     <t>a</t>
   </si>
   <si>
+    <t>PSR B2127+11C</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>PSR B1534+12</t>
+  </si>
+  <si>
+    <t>c-d</t>
+  </si>
+  <si>
+    <t>PSR J1518+4904</t>
+  </si>
+  <si>
     <t>nan</t>
   </si>
   <si>
-    <t>PSR B2127+11C</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>PSR B1534+12</t>
-  </si>
-  <si>
-    <t>c-d</t>
-  </si>
-  <si>
-    <t>PSR J1518+4904</t>
-  </si>
-  <si>
     <t>inf</t>
   </si>
   <si>
@@ -305,10 +308,7 @@
     <t>w</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>null</t>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -688,54 +688,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442A48F9-5C2A-0C4A-86C3-C8F48BDE0BAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BB1569-DFF6-7A42-B506-C2CFA3B63DB0}">
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection sqref="A1:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -743,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1.2312000000000001</v>
@@ -770,7 +773,7 @@
         <v>108</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L2">
         <v>1975</v>
@@ -869,16 +872,16 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>2.718</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G5">
         <v>40.9</v>
@@ -890,10 +893,10 @@
         <v>0.249</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L5">
         <v>1997</v>
@@ -907,19 +910,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>2.57</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G6">
         <v>104.2</v>
@@ -931,16 +934,16 @@
         <v>0.82799999999999996</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L6">
         <v>2001</v>
       </c>
       <c r="M6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -948,7 +951,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>1.1253</v>
@@ -975,13 +978,13 @@
         <v>204</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L7">
         <v>2003</v>
       </c>
       <c r="M7" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -989,19 +992,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>2.59</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G8">
         <v>41</v>
@@ -1013,10 +1016,10 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L8">
         <v>2004</v>
@@ -1030,7 +1033,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>1.1177999999999999</v>
@@ -1057,7 +1060,7 @@
         <v>443</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L9">
         <v>2005</v>
@@ -1071,19 +1074,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>2.59</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G10">
         <v>185.5</v>
@@ -1095,10 +1098,10 @@
         <v>0.39900000000000002</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L10">
         <v>2012</v>
@@ -1112,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>1.1754</v>
@@ -1136,16 +1139,16 @@
         <v>0.113</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L11">
         <v>2015</v>
       </c>
       <c r="M11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1153,7 +1156,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>1.2467999999999999</v>
@@ -1180,7 +1183,7 @@
         <v>2687</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L12">
         <v>2016</v>
@@ -1194,40 +1197,40 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>1.1879999999999999</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L13">
         <v>2017</v>
       </c>
       <c r="M13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1235,19 +1238,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <v>2.5379999999999998</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G14">
         <v>62.4</v>
@@ -1259,10 +1262,10 @@
         <v>0.1699</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L14">
         <v>2017</v>
@@ -1276,7 +1279,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15">
         <v>1.1893</v>
@@ -1300,10 +1303,10 @@
         <v>0.60599999999999998</v>
       </c>
       <c r="J15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L15">
         <v>2018</v>
@@ -1317,7 +1320,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16">
         <v>1.2174</v>
@@ -1344,7 +1347,7 @@
         <v>153</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L16">
         <v>2018</v>
@@ -1358,7 +1361,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>1.0882000000000001</v>
@@ -1385,7 +1388,7 @@
         <v>46</v>
       </c>
       <c r="K17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L17">
         <v>2018</v>
@@ -1399,7 +1402,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18">
         <v>1.44</v>
@@ -1408,47 +1411,47 @@
         <v>3.4</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L18">
         <v>2019</v>
       </c>
       <c r="M18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" location="a" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - a" xr:uid="{AEB02DE4-E3DE-1D4F-A74E-1E9A06947644}"/>
-    <hyperlink ref="K3" r:id="rId2" location="b" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - b" xr:uid="{5A856D82-1418-DB4E-810F-9128BD2D3606}"/>
-    <hyperlink ref="K8" r:id="rId3" location="k" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - k" xr:uid="{C8DEB56D-5990-4C41-B9CD-E172D8910F2A}"/>
-    <hyperlink ref="K9" r:id="rId4" location="l" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - l" xr:uid="{FABF8FB4-02A6-A649-A61C-3C2FCE3E723B}"/>
-    <hyperlink ref="K10" r:id="rId5" location="m" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - m" xr:uid="{0D05CCCB-47C2-E24B-9E1D-81EA3B94E713}"/>
-    <hyperlink ref="K11" r:id="rId6" location="n" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - n" xr:uid="{C25ACA41-B69B-7949-8CEA-E782158A4031}"/>
-    <hyperlink ref="K12" r:id="rId7" location="o" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - o" xr:uid="{B6C2BF07-C47B-A04E-82FD-A9A758610A10}"/>
-    <hyperlink ref="K13" r:id="rId8" location="p" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - p" xr:uid="{C397B457-2FB2-B043-9417-668B24118CFE}"/>
-    <hyperlink ref="K14" r:id="rId9" location="q" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - q" xr:uid="{EDA72F1E-5551-FD40-B5E8-C57A4554F835}"/>
-    <hyperlink ref="K15" r:id="rId10" location="r" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - r" xr:uid="{58090146-47D8-364A-B5D7-1FBB310D7585}"/>
-    <hyperlink ref="K16" r:id="rId11" location="t" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - t" xr:uid="{92F811C5-0050-344B-9F25-996C3D90F1D5}"/>
-    <hyperlink ref="K18" r:id="rId12" location="w" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - w" xr:uid="{79B26038-757B-5040-93C7-9C5ADC124354}"/>
+    <hyperlink ref="K2" r:id="rId1" location="a" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - a" xr:uid="{05599C17-8D64-DD44-828E-544F7045DF27}"/>
+    <hyperlink ref="K3" r:id="rId2" location="b" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - b" xr:uid="{26821E65-E82D-0647-87D4-F3062B22B929}"/>
+    <hyperlink ref="K8" r:id="rId3" location="k" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - k" xr:uid="{36AD361E-FD93-D742-9B62-C63392113AD2}"/>
+    <hyperlink ref="K9" r:id="rId4" location="l" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - l" xr:uid="{EFCD39D4-602E-874D-A7DE-EC219C548127}"/>
+    <hyperlink ref="K10" r:id="rId5" location="m" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - m" xr:uid="{C6611A52-BFEF-D346-97C2-F2BEC1248C2D}"/>
+    <hyperlink ref="K11" r:id="rId6" location="n" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - n" xr:uid="{125AAB29-ED38-0A45-A9EE-8C8BE413D0F2}"/>
+    <hyperlink ref="K12" r:id="rId7" location="o" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - o" xr:uid="{C277BFEA-AFC8-D14F-BDD6-111387063148}"/>
+    <hyperlink ref="K13" r:id="rId8" location="p" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - p" xr:uid="{C8FD936F-3F0C-0448-ADBD-A57B89960431}"/>
+    <hyperlink ref="K14" r:id="rId9" location="q" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - q" xr:uid="{0B23725D-2141-6F4A-8161-3FA646F0D2EE}"/>
+    <hyperlink ref="K15" r:id="rId10" location="r" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - r" xr:uid="{66437134-41E3-C441-A66A-BE272D91BB50}"/>
+    <hyperlink ref="K16" r:id="rId11" location="t" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - t" xr:uid="{6C6C1623-2FBC-E848-8353-1E80DA6BD715}"/>
+    <hyperlink ref="K18" r:id="rId12" location="w" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - w" xr:uid="{AEAD96F4-A5FA-0648-9CB8-CA70FDBC6BDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>